<commit_message>
Corrected error with passports
</commit_message>
<xml_diff>
--- a/Components.xlsx
+++ b/Components.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\source\repos\Warehouse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4798C4E-030F-46C1-B958-E9334C0CA9D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BFB323-B3F6-4D28-AB3B-A7263CD16F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1678,7 +1678,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X1" sqref="X1"/>
+      <selection pane="bottomLeft" activeCell="U162" sqref="U162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10200,23 +10200,33 @@
       <c r="D159" s="25">
         <v>0</v>
       </c>
-      <c r="E159" s="16"/>
+      <c r="E159" s="16">
+        <v>1</v>
+      </c>
       <c r="F159" s="16"/>
       <c r="G159" s="16"/>
       <c r="H159" s="5"/>
-      <c r="I159" s="15"/>
+      <c r="I159" s="15">
+        <v>1</v>
+      </c>
       <c r="J159" s="15"/>
       <c r="K159" s="15"/>
       <c r="L159" s="6"/>
-      <c r="M159" s="17"/>
+      <c r="M159" s="17">
+        <v>1</v>
+      </c>
       <c r="N159" s="17"/>
       <c r="O159" s="17"/>
       <c r="P159" s="17"/>
-      <c r="Q159" s="28"/>
+      <c r="Q159" s="28">
+        <v>1</v>
+      </c>
       <c r="R159" s="28"/>
       <c r="S159" s="28"/>
       <c r="T159" s="28"/>
-      <c r="U159" s="30"/>
+      <c r="U159" s="30">
+        <v>1</v>
+      </c>
       <c r="V159" s="30"/>
       <c r="W159" s="30"/>
       <c r="X159" s="30"/>
@@ -10235,23 +10245,33 @@
         <v>0</v>
       </c>
       <c r="E160" s="16"/>
-      <c r="F160" s="16"/>
+      <c r="F160" s="16">
+        <v>1</v>
+      </c>
       <c r="G160" s="16"/>
       <c r="H160" s="5"/>
       <c r="I160" s="15"/>
-      <c r="J160" s="15"/>
+      <c r="J160" s="15">
+        <v>1</v>
+      </c>
       <c r="K160" s="15"/>
       <c r="L160" s="6"/>
       <c r="M160" s="17"/>
-      <c r="N160" s="17"/>
+      <c r="N160" s="17">
+        <v>1</v>
+      </c>
       <c r="O160" s="17"/>
       <c r="P160" s="17"/>
       <c r="Q160" s="28"/>
-      <c r="R160" s="28"/>
+      <c r="R160" s="28">
+        <v>1</v>
+      </c>
       <c r="S160" s="28"/>
       <c r="T160" s="28"/>
       <c r="U160" s="30"/>
-      <c r="V160" s="30"/>
+      <c r="V160" s="30">
+        <v>1</v>
+      </c>
       <c r="W160" s="30"/>
       <c r="X160" s="30"/>
     </row>
@@ -10268,60 +10288,40 @@
       <c r="D161" s="20">
         <v>0</v>
       </c>
-      <c r="E161" s="16">
-        <v>1</v>
-      </c>
-      <c r="F161" s="16">
-        <v>1</v>
-      </c>
+      <c r="E161" s="16"/>
+      <c r="F161" s="16"/>
       <c r="G161" s="16">
         <v>1</v>
       </c>
       <c r="H161" s="16">
         <v>1</v>
       </c>
-      <c r="I161" s="15">
-        <v>1</v>
-      </c>
-      <c r="J161" s="15">
-        <v>1</v>
-      </c>
+      <c r="I161" s="15"/>
+      <c r="J161" s="15"/>
       <c r="K161" s="15">
         <v>1</v>
       </c>
       <c r="L161" s="15">
         <v>1</v>
       </c>
-      <c r="M161" s="17">
-        <v>1</v>
-      </c>
-      <c r="N161" s="17">
-        <v>1</v>
-      </c>
+      <c r="M161" s="17"/>
+      <c r="N161" s="17"/>
       <c r="O161" s="17">
         <v>1</v>
       </c>
       <c r="P161" s="17">
         <v>1</v>
       </c>
-      <c r="Q161" s="28">
-        <v>1</v>
-      </c>
-      <c r="R161" s="28">
-        <v>1</v>
-      </c>
+      <c r="Q161" s="28"/>
+      <c r="R161" s="28"/>
       <c r="S161" s="28">
         <v>1</v>
       </c>
       <c r="T161" s="28">
         <v>1</v>
       </c>
-      <c r="U161" s="30">
-        <v>1</v>
-      </c>
-      <c r="V161" s="30">
-        <v>1</v>
-      </c>
+      <c r="U161" s="30"/>
+      <c r="V161" s="30"/>
       <c r="W161" s="30">
         <v>1</v>
       </c>

</xml_diff>